<commit_message>
Generate test cases for test 'Login' test case
</commit_message>
<xml_diff>
--- a/data/test-data.xlsx
+++ b/data/test-data.xlsx
@@ -1,32 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\src\cortejo\test-data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{791D403F-1A88-4EE4-B527-DE40CED641D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="Calc"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="13" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
   </extLst>
 </workbook>
@@ -35,100 +22,123 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="22">
   <si>
-    <t>Login</t>
-  </si>
-  <si>
-    <t>Use Case</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>Input Elements</t>
-  </si>
-  <si>
-    <t>Action</t>
-  </si>
-  <si>
-    <t>Expected Result</t>
-  </si>
-  <si>
-    <t>Verify successful login with valid credentials.</t>
-  </si>
-  <si>
-    <t>Positive</t>
-  </si>
-  <si>
-    <t>Username: [Provide a valid username] Password: [Provide the corresponding valid password]</t>
-  </si>
-  <si>
-    <t>Click the "OK" button.</t>
-  </si>
-  <si>
-    <t>The page displays a menu with the id "menu", indicating a successful login.</t>
-  </si>
-  <si>
-    <t>Verify login fails with an invalid username.</t>
-  </si>
-  <si>
-    <t>Error</t>
-  </si>
-  <si>
-    <t>Username: [Provide an invalid username] Password: [Provide a valid password]</t>
-  </si>
-  <si>
-    <t>The page shows a message box with id "error-message" and the error text within "error-message-text".</t>
-  </si>
-  <si>
-    <t>Verify login fails with an invalid password.</t>
-  </si>
-  <si>
-    <t>Username: [Provide a valid username] Password: [Provide an invalid password]</t>
-  </si>
-  <si>
-    <t>Verify login fails with an empty username.</t>
-  </si>
-  <si>
-    <t>Username: [Leave the username field empty] Password: [Provide a valid password]</t>
-  </si>
-  <si>
-    <t>Verify login fails with an empty password.</t>
-  </si>
-  <si>
-    <t>Username: [Provide a valid username] Password: [Leave the password field empty]</t>
+    <t xml:space="preserve">Use Case</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Input Elements</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Action</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Expected Result</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Login</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify successful login with valid credentials.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Positive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Username: [Provide a valid username] Password: [Provide the corresponding valid password]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Click the "OK" button.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The page displays a menu with the id "menu", indicating a successful login.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify login fails with an invalid username.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Username: [Provide an invalid username] Password: [Provide a valid password]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The page shows a message box with id "error-message" and the error text within "error-message-text".</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify login fails with an invalid password.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Username: [Provide a valid username] Password: [Provide an invalid password]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify login fails with an empty username.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Username: [Leave the username field empty] Password: [Provide a valid password]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify login fails with an empty password.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Username: [Provide a valid username] Password: [Leave the password field empty]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="General"/>
+  </numFmts>
+  <fonts count="7">
     <font>
       <sz val="11"/>
-      <color indexed="8"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
     </font>
     <font>
       <sz val="11"/>
-      <color indexed="8"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
-      <b/>
+      <b val="true"/>
       <sz val="11.5"/>
       <color rgb="FFFFFFFF"/>
       <name val="Ubuntu"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="9.5"/>
-      <color indexed="8"/>
+      <color rgb="FF000000"/>
       <name val="Ubuntu"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -141,19 +151,19 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF999999"/>
-        <bgColor indexed="64"/>
+        <bgColor rgb="FF808080"/>
       </patternFill>
     </fill>
   </fills>
   <borders count="4">
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left style="medium">
         <color rgb="FFE3E3E3"/>
       </left>
@@ -166,7 +176,7 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left style="medium">
         <color rgb="FFE3E3E3"/>
       </left>
@@ -181,7 +191,7 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left style="medium">
         <color rgb="FFE3E3E3"/>
       </left>
@@ -193,304 +203,220 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFill="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFill="0" applyProtection="0"/>
+  <cellStyleXfs count="21">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Normal 2" xfId="20"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00CBD6DD"/>
-      <rgbColor rgb="00E5EAEE"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFE3E3E3"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF999999"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
     </indexedColors>
-    <mruColors>
-      <color rgb="FFE34317"/>
-      <color rgb="FFFF3300"/>
-    </mruColors>
   </colors>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:srgbClr val="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:srgbClr val="ffffff"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="44546a"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="e7e6e6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="4472c4"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="ed7d31"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="a5a5a5"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="ffc000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="5b9bd5"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="70ad47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="0563c1"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="954f72"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204" pitchFamily="0" charset="1"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="0" charset="1"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme>
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
                 <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
                 <a:tint val="67000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="50000">
               <a:schemeClr val="phClr">
                 <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
                 <a:tint val="73000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
                 <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
                 <a:tint val="81000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
+          <a:tileRect l="0" t="0" r="0" b="0"/>
         </a:gradFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
                 <a:lumMod val="102000"/>
                 <a:tint val="94000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
                 <a:lumMod val="100000"/>
                 <a:shade val="100000"/>
               </a:schemeClr>
@@ -498,33 +424,24 @@
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
                 <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
                 <a:shade val="78000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
+          <a:tileRect l="0" t="0" r="0" b="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
         <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
@@ -537,13 +454,7 @@
           <a:effectLst/>
         </a:effectStyle>
         <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
+          <a:effectLst/>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
@@ -553,15 +464,13 @@
         <a:solidFill>
           <a:schemeClr val="phClr">
             <a:tint val="95000"/>
-            <a:satMod val="170000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
                 <a:tint val="93000"/>
-                <a:satMod val="150000"/>
                 <a:shade val="98000"/>
                 <a:lumMod val="102000"/>
               </a:schemeClr>
@@ -569,7 +478,6 @@
             <a:gs pos="50000">
               <a:schemeClr val="phClr">
                 <a:tint val="98000"/>
-                <a:satMod val="130000"/>
                 <a:shade val="90000"/>
                 <a:lumMod val="103000"/>
               </a:schemeClr>
@@ -577,66 +485,62 @@
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
                 <a:shade val="63000"/>
-                <a:satMod val="120000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
+          <a:tileRect l="0" t="0" r="0" b="0"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB79D514-0BA8-4FC9-849F-A352069887A5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39" customWidth="1"/>
-    <col min="3" max="3" width="20.88671875" customWidth="1"/>
-    <col min="4" max="4" width="40.44140625" customWidth="1"/>
-    <col min="5" max="5" width="22.21875" customWidth="1"/>
-    <col min="6" max="6" width="66.77734375" customWidth="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="40.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="66.78"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="2" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
-        <v>0</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>7</v>
@@ -654,9 +558,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>12</v>
@@ -674,9 +578,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>16</v>
@@ -694,9 +598,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>18</v>
@@ -714,9 +618,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>20</v>
@@ -735,8 +639,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Added bounded context scope
</commit_message>
<xml_diff>
--- a/data/test-data.xlsx
+++ b/data/test-data.xlsx
@@ -20,7 +20,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="24">
+  <si>
+    <t xml:space="preserve">Bounded Context</t>
+  </si>
   <si>
     <t xml:space="preserve">Use Case</t>
   </si>
@@ -38,6 +41,9 @@
   </si>
   <si>
     <t xml:space="preserve">Expected Result</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Auth</t>
   </si>
   <si>
     <t xml:space="preserve">Login</t>
@@ -231,8 +237,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -502,140 +512,159 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="40.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="66.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="46.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="20.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="40.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="22.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="66.79"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+    <row r="1" customFormat="false" ht="27.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
-        <v>6</v>
+    <row r="2" customFormat="false" ht="22.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>7</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="22.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="B3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>11</v>
+      <c r="C3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>17</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4" t="s">
+    <row r="4" customFormat="false" ht="22.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="3" t="s">
+      <c r="G4" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="22.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>15</v>
       </c>
+      <c r="E5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="4" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="3" t="s">
+    <row r="6" customFormat="false" ht="22.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="4" t="s">
         <v>17</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added configurable url por Bounded Context
</commit_message>
<xml_diff>
--- a/data/test-data.xlsx
+++ b/data/test-data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="26">
   <si>
     <t xml:space="preserve">Bounded Context</t>
   </si>
@@ -34,6 +34,9 @@
     <t xml:space="preserve">Type</t>
   </si>
   <si>
+    <t xml:space="preserve">Skip Generation</t>
+  </si>
+  <si>
     <t xml:space="preserve">Input Elements</t>
   </si>
   <si>
@@ -53,6 +56,9 @@
   </si>
   <si>
     <t xml:space="preserve">Positive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes</t>
   </si>
   <si>
     <t xml:space="preserve">Username: [Provide a valid username] Password: [Provide the corresponding valid password]</t>
@@ -512,21 +518,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="20.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="46.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="20.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="40.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="22.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="66.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="40.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="22.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="66.79"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="27.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -548,123 +554,139 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="22.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>7</v>
+      <c r="A2" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="22.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>7</v>
+      <c r="A3" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>17</v>
+      <c r="H3" s="4" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="22.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>7</v>
+      <c r="A4" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" s="4" t="s">
         <v>19</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="22.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>7</v>
+      <c r="A5" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="22.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>7</v>
+      <c r="A6" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>23</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="E6" s="5"/>
       <c r="F6" s="4" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added prompt templates (by bounded context/use case and with default template)
</commit_message>
<xml_diff>
--- a/data/test-data.xlsx
+++ b/data/test-data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="26">
   <si>
     <t xml:space="preserve">Bounded Context</t>
   </si>
@@ -521,7 +521,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2:E5"/>
+      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -652,9 +652,7 @@
       <c r="D5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="4" t="s">
-        <v>12</v>
-      </c>
+      <c r="E5" s="4"/>
       <c r="F5" s="4" t="s">
         <v>23</v>
       </c>

</xml_diff>